<commit_message>
plots and report added
</commit_message>
<xml_diff>
--- a/Sizing_sheet.xlsx
+++ b/Sizing_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achin\Software\IIITB\Semester_7\ACMOS\Flipped-Voltage-Follower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5D36E14-AF7C-4776-8B9D-B7FD0C3A0402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F489EC28-FCCE-4CEE-8C28-31C854782CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Step 1: List Down the Specifications and classify them</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>(Cc+Cgd)-Cgd</t>
+  </si>
+  <si>
+    <t>FVF Sizing</t>
+  </si>
+  <si>
+    <t>Ibias</t>
+  </si>
+  <si>
+    <t>From PMOS techplots: Choose higher, a little overdesigned</t>
+  </si>
+  <si>
+    <t>From PMOS techplots</t>
   </si>
 </sst>
 </file>
@@ -816,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F83"/>
+  <dimension ref="B3:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1536,6 +1548,139 @@
       </c>
       <c r="F83" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" s="10" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B86" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="13"/>
+    </row>
+    <row r="87" spans="2:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88">
+        <v>10</v>
+      </c>
+      <c r="F88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89">
+        <f>50/1000000</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90">
+        <v>62.6</v>
+      </c>
+      <c r="F90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B91" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="F91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92">
+        <v>2.59</v>
+      </c>
+      <c r="F92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B93" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3">
+        <f>1000000*D89/D92</f>
+        <v>19.305019305019307</v>
+      </c>
+      <c r="F93" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94">
+        <f>D88*D89</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F94" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>25</v>
+      </c>
+      <c r="D95">
+        <f>D90/D94</f>
+        <v>125200</v>
+      </c>
+      <c r="F95" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <f>ATAN(D53*D18/D49)</f>
+        <v>0.53815398534274816</v>
+      </c>
+      <c r="E99">
+        <f>180/3.14*D99</f>
+        <v>30.849591516463267</v>
+      </c>
+      <c r="F99">
+        <f>90-E99</f>
+        <v>59.150408483536737</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <f>ATAN(D53*D18/D48)</f>
+        <v>0.22305631015390384</v>
+      </c>
+      <c r="E100">
+        <f>180/3.14*D100</f>
+        <v>12.786667461051811</v>
+      </c>
+      <c r="F100">
+        <f>90-E100</f>
+        <v>77.213332538948194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>